<commit_message>
Parts edits, adding notes tracking history of activity, capturing context and investigations through-out the build
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\zelda-master-sword\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69EF6B6-E690-47A7-8F69-E7024BAE4A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC3D9DD-4CD4-4629-80AF-A666ED28B7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{71EF3422-4AEF-49A3-9F8A-3093471F385F}"/>
+    <workbookView xWindow="0" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{71EF3422-4AEF-49A3-9F8A-3093471F385F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
   <si>
     <t>Anchor Pin.stl</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>transparent green</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -515,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E251D61-DDCB-4785-A50E-3C55030DDF72}">
-  <dimension ref="A2:C25"/>
+  <dimension ref="A2:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +531,7 @@
     <col min="6" max="6" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -538,8 +541,11 @@
       <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -550,7 +556,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -561,7 +567,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -572,7 +578,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -583,7 +589,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -594,7 +600,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -605,7 +611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -616,7 +622,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -627,7 +633,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -635,7 +641,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -643,7 +649,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -654,7 +660,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -662,7 +668,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -673,7 +679,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
BOM edits.  Added link to video from Overture folks showing Luminous Blue HS TPU glows in the dark!
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\zelda-master-sword\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC3D9DD-4CD4-4629-80AF-A666ED28B7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E575EEF7-5637-4915-BACC-213869F18CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{71EF3422-4AEF-49A3-9F8A-3093471F385F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
   <si>
     <t>Anchor Pin.stl</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Army Purple</t>
   </si>
 </sst>
 </file>
@@ -521,7 +524,7 @@
   <dimension ref="A2:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,6 +643,9 @@
       <c r="B11" t="s">
         <v>27</v>
       </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -648,6 +654,9 @@
       <c r="B12" t="s">
         <v>27</v>
       </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -667,6 +676,9 @@
       <c r="B14" t="s">
         <v>27</v>
       </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -730,6 +742,9 @@
       <c r="B20" t="s">
         <v>27</v>
       </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -771,6 +786,9 @@
       <c r="B24" t="s">
         <v>27</v>
       </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -778,6 +796,9 @@
       </c>
       <c r="B25" t="s">
         <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>